<commit_message>
Renamed few trancripts. Updated the DataSheet
</commit_message>
<xml_diff>
--- a/data/Subset 1/7th grade math.xlsx
+++ b/data/Subset 1/7th grade math.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Teacher Tag</t>
+          <t>T Tag</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -475,7 +475,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -500,7 +500,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -525,7 +525,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -550,7 +550,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -575,7 +575,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -600,7 +600,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -625,7 +625,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -650,7 +650,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -675,7 +675,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -725,7 +725,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -750,7 +750,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -775,7 +775,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -800,7 +800,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -825,7 +825,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -850,7 +850,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -875,7 +875,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -900,7 +900,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -950,7 +950,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>STUDENT</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -975,7 +975,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>STUDENT</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1025,7 +1025,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1050,7 +1050,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1100,7 +1100,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1275,7 +1275,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1350,7 +1350,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1425,7 +1425,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1450,7 +1450,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1625,7 +1625,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1700,7 +1700,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>STUDENT</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1850,7 +1850,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>STUDENT</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1875,7 +1875,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -1900,7 +1900,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -1950,7 +1950,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>STUDENT</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -1975,7 +1975,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>STUDENT</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2025,7 +2025,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2075,7 +2075,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2100,7 +2100,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2125,7 +2125,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2150,7 +2150,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>STUDENT</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2175,7 +2175,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2200,7 +2200,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2250,7 +2250,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2300,7 +2300,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2325,7 +2325,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2350,7 +2350,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2375,7 +2375,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -2450,7 +2450,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>STUDENT</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -2475,7 +2475,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2500,7 +2500,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2525,7 +2525,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2550,7 +2550,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2575,7 +2575,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2625,7 +2625,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -2700,7 +2700,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -2725,7 +2725,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -2750,7 +2750,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>STUDENT</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -2800,7 +2800,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -2850,7 +2850,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -2875,7 +2875,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -2900,7 +2900,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -2925,7 +2925,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -2950,7 +2950,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -2975,7 +2975,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>STUDENT</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -3000,7 +3000,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>TEACHER</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -3025,7 +3025,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>STUDENT</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -3050,7 +3050,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>TEACHER</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -3075,7 +3075,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>TEACHER</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -3150,7 +3150,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -3175,7 +3175,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -3200,7 +3200,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>STUDENT</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -3225,7 +3225,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -3250,7 +3250,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -3275,7 +3275,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -3300,7 +3300,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -3325,7 +3325,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -3350,7 +3350,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -3375,7 +3375,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -3450,7 +3450,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -3475,7 +3475,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -3500,7 +3500,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>STUDENTS</t>
+          <t>SS</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -3550,7 +3550,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -3575,7 +3575,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -3600,7 +3600,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -3625,7 +3625,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -3650,7 +3650,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -3675,7 +3675,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -3700,7 +3700,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -3725,7 +3725,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -3775,7 +3775,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -3800,7 +3800,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -3850,7 +3850,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -3875,7 +3875,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -3900,7 +3900,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -3925,7 +3925,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -3950,7 +3950,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -3975,7 +3975,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -4000,7 +4000,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>ANTOINETTE VILLARIN</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">

</xml_diff>